<commit_message>
Initial GMT case study. Full interaction w/ Excel. New case_study_params
</commit_message>
<xml_diff>
--- a/excel/local_calculations.xlsx
+++ b/excel/local_calculations.xlsx
@@ -909,8 +909,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:M41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A39" sqref="A39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -973,6 +973,9 @@
       <c r="C7" s="19" t="s">
         <v>20</v>
       </c>
+      <c r="F7">
+        <v>237</v>
+      </c>
       <c r="K7" s="1"/>
       <c r="L7" t="s">
         <v>35</v>
@@ -1064,7 +1067,6 @@
         <v>44</v>
       </c>
       <c r="B14" s="18">
-        <f>B9/2</f>
         <v>4.25</v>
       </c>
       <c r="C14" s="19" t="s">
@@ -1076,7 +1078,6 @@
         <v>39</v>
       </c>
       <c r="B15" s="18">
-        <f>B7/2</f>
         <v>118.5</v>
       </c>
       <c r="C15" s="19" t="s">

</xml_diff>

<commit_message>
Updated Excel Models, Local Solvers, Dump pre-revamp
</commit_message>
<xml_diff>
--- a/excel/local_calculations.xlsx
+++ b/excel/local_calculations.xlsx
@@ -9,12 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11085" windowHeight="7935"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11088" windowHeight="7932" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="NAVARCH" sheetId="1" r:id="rId1"/>
     <sheet name="DIST" sheetId="2" r:id="rId2"/>
     <sheet name="OPS" sheetId="3" r:id="rId3"/>
+    <sheet name="OPS (2)" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="130">
   <si>
     <t>kg/m^3</t>
   </si>
@@ -355,6 +356,78 @@
   </si>
   <si>
     <t>Density of Water</t>
+  </si>
+  <si>
+    <t>Given # of units, return sortie rates, durations etc/</t>
+  </si>
+  <si>
+    <t>Flight Time</t>
+  </si>
+  <si>
+    <t>Maintenance Time</t>
+  </si>
+  <si>
+    <t>Distance to Target</t>
+  </si>
+  <si>
+    <t>Average Cruise Speed</t>
+  </si>
+  <si>
+    <t>hrs</t>
+  </si>
+  <si>
+    <t>nm</t>
+  </si>
+  <si>
+    <t>kts (nm/hr)</t>
+  </si>
+  <si>
+    <t>Cruise Speed (kts)</t>
+  </si>
+  <si>
+    <t>Combat Radius (nm)</t>
+  </si>
+  <si>
+    <t>V_fuel</t>
+  </si>
+  <si>
+    <t>Tank Capacity (m^3)</t>
+  </si>
+  <si>
+    <t>SR</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>S</t>
+  </si>
+  <si>
+    <t>RFT</t>
+  </si>
+  <si>
+    <t>Volume Flow Rate:</t>
+  </si>
+  <si>
+    <t>Requirements:</t>
+  </si>
+  <si>
+    <t># Vehicles</t>
+  </si>
+  <si>
+    <t>**The vessel shall be able to support x number of vehicles for y number of days, with a sortie rate for each vehicle of z per day</t>
+  </si>
+  <si>
+    <t>Fuel Capacity (m^3)</t>
+  </si>
+  <si>
+    <t>Required Refueling Time (mins)</t>
+  </si>
+  <si>
+    <t>Required Flow Rate (m^3/s)</t>
+  </si>
+  <si>
+    <t>* Performance Based. The vessel shall be able to engage targets at a distance of x within y minutes</t>
   </si>
 </sst>
 </file>
@@ -909,26 +982,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:M41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A39" sqref="A39"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C42" sqref="C42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.5703125" customWidth="1"/>
-    <col min="2" max="2" width="15.85546875" customWidth="1"/>
-    <col min="3" max="3" width="15.42578125" customWidth="1"/>
-    <col min="4" max="4" width="15.85546875" customWidth="1"/>
+    <col min="1" max="1" width="20.5546875" customWidth="1"/>
+    <col min="2" max="2" width="15.88671875" customWidth="1"/>
+    <col min="3" max="3" width="15.44140625" customWidth="1"/>
+    <col min="4" max="4" width="15.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" s="14" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="15"/>
       <c r="C2" s="16"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" s="24" t="s">
         <v>3</v>
       </c>
@@ -942,7 +1015,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>105</v>
       </c>
@@ -953,7 +1026,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" s="14" t="s">
         <v>12</v>
       </c>
@@ -963,7 +1036,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" s="17" t="s">
         <v>15</v>
       </c>
@@ -981,7 +1054,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" s="17" t="s">
         <v>13</v>
       </c>
@@ -996,7 +1069,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" s="17" t="s">
         <v>14</v>
       </c>
@@ -1011,7 +1084,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" s="17" t="s">
         <v>19</v>
       </c>
@@ -1022,7 +1095,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11" s="17" t="s">
         <v>21</v>
       </c>
@@ -1034,7 +1107,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12" s="17" t="s">
         <v>33</v>
       </c>
@@ -1048,7 +1121,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13" s="17" t="s">
         <v>43</v>
       </c>
@@ -1062,7 +1135,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14" s="17" t="s">
         <v>44</v>
       </c>
@@ -1073,7 +1146,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15" s="17" t="s">
         <v>39</v>
       </c>
@@ -1084,7 +1157,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16" s="21" t="s">
         <v>23</v>
       </c>
@@ -1096,10 +1169,10 @@
         <v>24</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A17" s="3"/>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A18" s="27"/>
       <c r="B18" s="15" t="s">
         <v>6</v>
@@ -1120,7 +1193,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A19" s="28" t="s">
         <v>40</v>
       </c>
@@ -1144,7 +1217,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A20" s="31"/>
       <c r="B20" s="32"/>
       <c r="C20" s="32"/>
@@ -1153,7 +1226,7 @@
       <c r="L20" s="2"/>
       <c r="M20" s="2"/>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A21" s="31" t="s">
         <v>16</v>
       </c>
@@ -1161,7 +1234,7 @@
       <c r="C21" s="32"/>
       <c r="D21" s="33"/>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A22" s="34" t="s">
         <v>25</v>
       </c>
@@ -1175,7 +1248,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A23" s="34" t="s">
         <v>26</v>
       </c>
@@ -1186,7 +1259,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A24" s="34" t="s">
         <v>27</v>
       </c>
@@ -1203,7 +1276,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A25" s="28" t="s">
         <v>28</v>
       </c>
@@ -1220,13 +1293,13 @@
         <v>11</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A26" s="31"/>
       <c r="B26" s="32"/>
       <c r="C26" s="32"/>
       <c r="D26" s="33"/>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A27" s="21" t="s">
         <v>9</v>
       </c>
@@ -1243,10 +1316,10 @@
         <v>10.295362803977552</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B28" s="9"/>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
         <v>29</v>
       </c>
@@ -1265,7 +1338,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>45</v>
       </c>
@@ -1274,7 +1347,7 @@
         <v>-4.5362803977551991E-2</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>46</v>
       </c>
@@ -1283,7 +1356,7 @@
         <v>173.95463719602245</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
         <v>38</v>
       </c>
@@ -1295,12 +1368,12 @@
         <v>47</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" s="3" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" s="4" t="s">
         <v>4</v>
       </c>
@@ -1314,7 +1387,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" s="10"/>
       <c r="B39">
         <f>A39*$B$3/1000</f>
@@ -1330,7 +1403,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41" s="3"/>
     </row>
   </sheetData>
@@ -1346,19 +1419,19 @@
       <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="4" width="20.7109375" customWidth="1"/>
+    <col min="1" max="4" width="20.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="14" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="15"/>
       <c r="C2" s="16"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="31" t="s">
         <v>3</v>
       </c>
@@ -1369,7 +1442,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>101</v>
       </c>
@@ -1377,7 +1450,7 @@
         <v>9.81</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="24" t="s">
         <v>75</v>
       </c>
@@ -1389,14 +1462,14 @@
         <v>76</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="14" t="s">
         <v>99</v>
       </c>
       <c r="B7" s="15"/>
       <c r="C7" s="16"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="31" t="s">
         <v>86</v>
       </c>
@@ -1407,7 +1480,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="31" t="s">
         <v>87</v>
       </c>
@@ -1416,7 +1489,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="24" t="s">
         <v>88</v>
       </c>
@@ -1428,7 +1501,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="53" t="s">
         <v>102</v>
       </c>
@@ -1437,7 +1510,7 @@
         <v>3.1415926535897931</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="14" t="s">
         <v>98</v>
       </c>
@@ -1445,13 +1518,13 @@
       <c r="C12" s="15"/>
       <c r="D12" s="16"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="31"/>
       <c r="B13" s="45"/>
       <c r="C13" s="45"/>
       <c r="D13" s="19"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="31" t="s">
         <v>77</v>
       </c>
@@ -1461,7 +1534,7 @@
       </c>
       <c r="D14" s="19"/>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="31" t="s">
         <v>80</v>
       </c>
@@ -1475,7 +1548,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="31" t="s">
         <v>82</v>
       </c>
@@ -1485,7 +1558,7 @@
       </c>
       <c r="D16" s="48"/>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="31" t="s">
         <v>84</v>
       </c>
@@ -1500,13 +1573,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="31"/>
       <c r="B18" s="45"/>
       <c r="C18" s="45"/>
       <c r="D18" s="19"/>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="21" t="s">
         <v>79</v>
       </c>
@@ -1519,7 +1592,7 @@
       </c>
       <c r="D19" s="26"/>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>100</v>
       </c>
@@ -1531,12 +1604,12 @@
         <v>90</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" s="3" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B26" t="s">
         <v>96</v>
       </c>
@@ -1547,7 +1620,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>92</v>
       </c>
@@ -1561,7 +1634,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>93</v>
       </c>
@@ -1575,7 +1648,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>94</v>
       </c>
@@ -1589,7 +1662,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>95</v>
       </c>
@@ -1616,24 +1689,24 @@
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="25.28515625" customWidth="1"/>
-    <col min="2" max="3" width="20.42578125" customWidth="1"/>
-    <col min="4" max="4" width="26.42578125" customWidth="1"/>
+    <col min="1" max="1" width="25.33203125" customWidth="1"/>
+    <col min="2" max="3" width="20.44140625" customWidth="1"/>
+    <col min="4" max="4" width="26.44140625" customWidth="1"/>
     <col min="5" max="5" width="26" customWidth="1"/>
-    <col min="6" max="6" width="16.7109375" customWidth="1"/>
-    <col min="14" max="14" width="15.85546875" customWidth="1"/>
+    <col min="6" max="6" width="16.6640625" customWidth="1"/>
+    <col min="14" max="14" width="15.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="14" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="15"/>
       <c r="C2" s="16"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="24" t="s">
         <v>3</v>
       </c>
@@ -1647,7 +1720,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>51</v>
       </c>
@@ -1664,7 +1737,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>66</v>
       </c>
@@ -1682,7 +1755,7 @@
         <v>13.297052154195011</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>48</v>
       </c>
@@ -1700,7 +1773,7 @@
         <v>15.029478458049885</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>49</v>
       </c>
@@ -1721,7 +1794,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>50</v>
       </c>
@@ -1742,7 +1815,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B11" s="2" t="s">
         <v>54</v>
       </c>
@@ -1754,7 +1827,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
         <v>7</v>
       </c>
@@ -1762,7 +1835,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>74</v>
       </c>
@@ -1773,7 +1846,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
         <v>64</v>
       </c>
@@ -1781,7 +1854,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>55</v>
       </c>
@@ -1795,7 +1868,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>58</v>
       </c>
@@ -1806,7 +1879,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>63</v>
       </c>
@@ -1817,7 +1890,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>62</v>
       </c>
@@ -1828,7 +1901,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>69</v>
       </c>
@@ -1839,7 +1912,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>71</v>
       </c>
@@ -1851,7 +1924,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>72</v>
       </c>
@@ -1871,4 +1944,944 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:N59"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="B60" sqref="B60"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="25.33203125" customWidth="1"/>
+    <col min="2" max="3" width="20.44140625" customWidth="1"/>
+    <col min="4" max="4" width="26.44140625" customWidth="1"/>
+    <col min="5" max="5" width="26" customWidth="1"/>
+    <col min="6" max="6" width="20.21875" customWidth="1"/>
+    <col min="7" max="7" width="19" customWidth="1"/>
+    <col min="8" max="8" width="12.21875" customWidth="1"/>
+    <col min="9" max="9" width="15.6640625" customWidth="1"/>
+    <col min="10" max="10" width="14.21875" customWidth="1"/>
+    <col min="11" max="11" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.88671875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A2" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="15"/>
+      <c r="C2" s="16"/>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A3" s="24" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="25">
+        <v>845</v>
+      </c>
+      <c r="C3" s="26" t="s">
+        <v>0</v>
+      </c>
+      <c r="E3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A5" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B5" t="s">
+        <v>52</v>
+      </c>
+      <c r="C5" t="s">
+        <v>103</v>
+      </c>
+      <c r="D5" t="s">
+        <v>53</v>
+      </c>
+      <c r="E5" t="s">
+        <v>104</v>
+      </c>
+      <c r="F5" t="s">
+        <v>115</v>
+      </c>
+      <c r="G5" t="s">
+        <v>114</v>
+      </c>
+      <c r="H5" t="s">
+        <v>107</v>
+      </c>
+      <c r="I5" t="s">
+        <v>108</v>
+      </c>
+      <c r="J5" t="s">
+        <v>55</v>
+      </c>
+      <c r="K5" t="s">
+        <v>116</v>
+      </c>
+      <c r="L5" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>66</v>
+      </c>
+      <c r="B6" s="52">
+        <v>13.297052154195011</v>
+      </c>
+      <c r="C6" s="9">
+        <v>113.37868480725623</v>
+      </c>
+      <c r="D6" s="20">
+        <v>1</v>
+      </c>
+      <c r="E6" s="9">
+        <f>B6*D6</f>
+        <v>13.297052154195011</v>
+      </c>
+      <c r="F6">
+        <v>600</v>
+      </c>
+      <c r="G6">
+        <v>567</v>
+      </c>
+      <c r="H6">
+        <f>2*F6/G6</f>
+        <v>2.1164021164021163</v>
+      </c>
+      <c r="I6">
+        <f>3.4+0.64*H6</f>
+        <v>4.7544973544973548</v>
+      </c>
+      <c r="J6">
+        <f>24/(H6+I6+B19/60)</f>
+        <v>3.2560476634843156</v>
+      </c>
+      <c r="K6">
+        <f>J6*D6*$B$21*H6*C6*60/$B$3</f>
+        <v>554.77246436455914</v>
+      </c>
+      <c r="L6">
+        <f>H6*60*C6/$B$3</f>
+        <v>17.038216933559685</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>48</v>
+      </c>
+      <c r="B7" s="52">
+        <v>15.029478458049885</v>
+      </c>
+      <c r="C7" s="9">
+        <v>40.816326530612244</v>
+      </c>
+      <c r="D7" s="20">
+        <v>1</v>
+      </c>
+      <c r="E7" s="9">
+        <f t="shared" ref="E7:E9" si="0">B7*D7</f>
+        <v>15.029478458049885</v>
+      </c>
+      <c r="F7">
+        <v>428</v>
+      </c>
+      <c r="G7">
+        <v>270</v>
+      </c>
+      <c r="H7">
+        <f t="shared" ref="H7:H10" si="1">2*F7/G7</f>
+        <v>3.1703703703703705</v>
+      </c>
+      <c r="I7">
+        <f t="shared" ref="I7:I9" si="2">3.4+0.64*H7</f>
+        <v>5.4290370370370375</v>
+      </c>
+      <c r="J7">
+        <f t="shared" ref="J7:J9" si="3">24/(H7+I7+B20/60)</f>
+        <v>0.94989035216305273</v>
+      </c>
+      <c r="K7">
+        <f t="shared" ref="K7:K9" si="4">J7*D7*$B$21*H7*C7*60/$B$3</f>
+        <v>87.279436616787891</v>
+      </c>
+      <c r="L7">
+        <f>H7*60*C7/$B$3</f>
+        <v>9.1883696279300668</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>49</v>
+      </c>
+      <c r="B8" s="52">
+        <v>6.7437641723356005</v>
+      </c>
+      <c r="C8" s="9">
+        <v>95.238095238095241</v>
+      </c>
+      <c r="D8" s="20">
+        <v>1</v>
+      </c>
+      <c r="E8" s="9">
+        <f t="shared" si="0"/>
+        <v>6.7437641723356005</v>
+      </c>
+      <c r="F8" s="41">
+        <v>300</v>
+      </c>
+      <c r="G8">
+        <v>550</v>
+      </c>
+      <c r="H8">
+        <f t="shared" si="1"/>
+        <v>1.0909090909090908</v>
+      </c>
+      <c r="I8">
+        <f t="shared" si="2"/>
+        <v>4.0981818181818177</v>
+      </c>
+      <c r="J8">
+        <f t="shared" si="3"/>
+        <v>4.4811587642865227</v>
+      </c>
+      <c r="K8">
+        <f>J8*D8*$B$21*H8*C8*60/$B$3</f>
+        <v>330.58575376278043</v>
+      </c>
+      <c r="L8">
+        <f>H8*60*C8/$B$3</f>
+        <v>7.3772381464689163</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>50</v>
+      </c>
+      <c r="B9" s="52">
+        <v>8.0535147392290245</v>
+      </c>
+      <c r="C9" s="9">
+        <v>8.2993197278911559</v>
+      </c>
+      <c r="D9" s="20">
+        <v>1</v>
+      </c>
+      <c r="E9" s="9">
+        <f t="shared" si="0"/>
+        <v>8.0535147392290245</v>
+      </c>
+      <c r="F9" s="41">
+        <v>225</v>
+      </c>
+      <c r="G9">
+        <v>91</v>
+      </c>
+      <c r="H9">
+        <f t="shared" si="1"/>
+        <v>4.9450549450549453</v>
+      </c>
+      <c r="I9">
+        <f t="shared" si="2"/>
+        <v>6.5648351648351646</v>
+      </c>
+      <c r="J9">
+        <f t="shared" si="3"/>
+        <v>2.0851632614092037</v>
+      </c>
+      <c r="K9">
+        <f t="shared" si="4"/>
+        <v>60.764261390825958</v>
+      </c>
+      <c r="L9">
+        <f>H9*60*C9/$B$3</f>
+        <v>2.9141248800710216</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B11" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C11" s="54">
+        <f>SUM(E6:E9)</f>
+        <v>43.12380952380952</v>
+      </c>
+      <c r="D11" t="s">
+        <v>10</v>
+      </c>
+      <c r="K11">
+        <f>SUM(K6:K9)</f>
+        <v>1033.4019161349534</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B13" t="s">
+        <v>7</v>
+      </c>
+      <c r="C13" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A14" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B14" s="44">
+        <v>50</v>
+      </c>
+      <c r="C14" s="44">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A16" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="B16" s="41" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>55</v>
+      </c>
+      <c r="B17" s="1">
+        <v>2</v>
+      </c>
+      <c r="C17" t="s">
+        <v>56</v>
+      </c>
+      <c r="D17" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>58</v>
+      </c>
+      <c r="B18" s="1">
+        <v>60</v>
+      </c>
+      <c r="C18" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>63</v>
+      </c>
+      <c r="B19" s="1">
+        <v>30</v>
+      </c>
+      <c r="C19" t="s">
+        <v>60</v>
+      </c>
+      <c r="G19">
+        <f>24/$B$17 - H6-I6</f>
+        <v>5.129100529100528</v>
+      </c>
+      <c r="H19">
+        <f>G19-150/60</f>
+        <v>2.629100529100528</v>
+      </c>
+      <c r="I19">
+        <f>H19*60</f>
+        <v>157.74603174603169</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>62</v>
+      </c>
+      <c r="B20" s="1">
+        <v>1000</v>
+      </c>
+      <c r="C20" t="s">
+        <v>61</v>
+      </c>
+      <c r="G20">
+        <f t="shared" ref="G20:G22" si="5">24/$B$17 - H7-I7</f>
+        <v>3.4005925925925915</v>
+      </c>
+      <c r="H20">
+        <f t="shared" ref="H20:H22" si="6">G20-150/60</f>
+        <v>0.9005925925925915</v>
+      </c>
+      <c r="I20">
+        <f t="shared" ref="I20:I22" si="7">H20*60</f>
+        <v>54.03555555555549</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>69</v>
+      </c>
+      <c r="B21" s="1">
+        <v>10</v>
+      </c>
+      <c r="C21" t="s">
+        <v>70</v>
+      </c>
+      <c r="G21">
+        <f t="shared" si="5"/>
+        <v>6.8109090909090924</v>
+      </c>
+      <c r="H21">
+        <f t="shared" si="6"/>
+        <v>4.3109090909090924</v>
+      </c>
+      <c r="I21">
+        <f t="shared" si="7"/>
+        <v>258.65454545454554</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="G22">
+        <f t="shared" si="5"/>
+        <v>0.49010989010989015</v>
+      </c>
+      <c r="H22">
+        <f t="shared" si="6"/>
+        <v>-2.0098901098901099</v>
+      </c>
+      <c r="I22">
+        <f t="shared" si="7"/>
+        <v>-120.5934065934066</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A23" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B23" s="44">
+        <f>B17*B18*B21*SUMPRODUCT(C6:C9,D6:D9)/B3</f>
+        <v>366.01054623032644</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A24" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B24" s="43">
+        <f>B20*B19/2.205/B3/60</f>
+        <v>0.26835191670356501</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="D24" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>55</v>
+      </c>
+      <c r="B28">
+        <f>24/(B31+B32+B33)</f>
+        <v>3.5820895522388061</v>
+      </c>
+      <c r="E28" t="s">
+        <v>118</v>
+      </c>
+      <c r="F28">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>109</v>
+      </c>
+      <c r="B29">
+        <v>500</v>
+      </c>
+      <c r="C29" t="s">
+        <v>112</v>
+      </c>
+      <c r="E29" t="s">
+        <v>119</v>
+      </c>
+      <c r="F29">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>110</v>
+      </c>
+      <c r="B30">
+        <v>600</v>
+      </c>
+      <c r="C30" t="s">
+        <v>113</v>
+      </c>
+      <c r="E30" t="s">
+        <v>120</v>
+      </c>
+      <c r="F30">
+        <v>567</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>107</v>
+      </c>
+      <c r="B31">
+        <f>2*B29/B30</f>
+        <v>1.6666666666666667</v>
+      </c>
+      <c r="C31" t="s">
+        <v>111</v>
+      </c>
+      <c r="E31" t="s">
+        <v>121</v>
+      </c>
+      <c r="F31">
+        <f>24/F28 - 3.36*(F29/F30) - 5.9</f>
+        <v>2.5444444444444443</v>
+      </c>
+      <c r="G31" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>63</v>
+      </c>
+      <c r="B32">
+        <v>0.5</v>
+      </c>
+      <c r="C32" t="s">
+        <v>111</v>
+      </c>
+      <c r="F32">
+        <f>F31*60</f>
+        <v>152.66666666666666</v>
+      </c>
+      <c r="G32" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>108</v>
+      </c>
+      <c r="B33">
+        <f>3.4+0.68*B31</f>
+        <v>4.5333333333333332</v>
+      </c>
+      <c r="C33" t="s">
+        <v>111</v>
+      </c>
+      <c r="E33" t="s">
+        <v>122</v>
+      </c>
+      <c r="F33">
+        <f>L6/F32*60</f>
+        <v>6.696242462971056</v>
+      </c>
+      <c r="G33" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14" ht="7.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="15"/>
+      <c r="B36" s="15"/>
+      <c r="C36" s="15"/>
+      <c r="D36" s="15"/>
+      <c r="E36" s="15"/>
+      <c r="F36" s="15"/>
+      <c r="G36" s="15"/>
+      <c r="H36" s="15"/>
+      <c r="I36" s="15"/>
+      <c r="J36" s="15"/>
+      <c r="K36" s="15"/>
+      <c r="L36" s="15"/>
+      <c r="M36" s="15"/>
+      <c r="N36" s="15"/>
+    </row>
+    <row r="37" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>123</v>
+      </c>
+      <c r="B37" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>69</v>
+      </c>
+      <c r="B39" s="20">
+        <v>10</v>
+      </c>
+      <c r="C39" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="40" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>55</v>
+      </c>
+      <c r="B40" s="20">
+        <v>2</v>
+      </c>
+      <c r="C40" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="43" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A43" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="B43" s="15"/>
+      <c r="C43" s="16"/>
+    </row>
+    <row r="44" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A44" s="24" t="s">
+        <v>3</v>
+      </c>
+      <c r="B44" s="46">
+        <v>845</v>
+      </c>
+      <c r="C44" s="26" t="s">
+        <v>0</v>
+      </c>
+      <c r="E44" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A46" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B46" t="s">
+        <v>52</v>
+      </c>
+      <c r="C46" t="s">
+        <v>103</v>
+      </c>
+      <c r="D46" t="s">
+        <v>53</v>
+      </c>
+      <c r="E46" t="s">
+        <v>104</v>
+      </c>
+      <c r="F46" t="s">
+        <v>115</v>
+      </c>
+      <c r="G46" t="s">
+        <v>114</v>
+      </c>
+      <c r="H46" t="s">
+        <v>126</v>
+      </c>
+      <c r="I46" t="s">
+        <v>107</v>
+      </c>
+      <c r="J46" t="s">
+        <v>108</v>
+      </c>
+      <c r="K46" t="s">
+        <v>116</v>
+      </c>
+      <c r="L46" t="s">
+        <v>127</v>
+      </c>
+      <c r="M46" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="47" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>66</v>
+      </c>
+      <c r="B47" s="52">
+        <v>13.297052154195011</v>
+      </c>
+      <c r="C47" s="9">
+        <v>113.37868480725623</v>
+      </c>
+      <c r="D47" s="20">
+        <v>1</v>
+      </c>
+      <c r="E47" s="9">
+        <f>B47*D47</f>
+        <v>13.297052154195011</v>
+      </c>
+      <c r="F47">
+        <v>600</v>
+      </c>
+      <c r="G47">
+        <v>567</v>
+      </c>
+      <c r="H47" s="9">
+        <f>I47*60*C47/$B$44</f>
+        <v>17.038216933559685</v>
+      </c>
+      <c r="I47" s="9">
+        <f>2*F47/G47</f>
+        <v>2.1164021164021163</v>
+      </c>
+      <c r="J47" s="9">
+        <f>3.4+0.64*I47</f>
+        <v>4.7544973544973548</v>
+      </c>
+      <c r="K47" s="9">
+        <f>$B$40*D47*$B$39*I47*C47*60/$B$3</f>
+        <v>340.76433867119368</v>
+      </c>
+      <c r="L47" s="9">
+        <f>60*(24/$B$40 - 3.36*(F47/G47) - 5.9)</f>
+        <v>152.66666666666666</v>
+      </c>
+      <c r="M47" s="9">
+        <f>H47/L47*60</f>
+        <v>6.696242462971056</v>
+      </c>
+    </row>
+    <row r="48" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>48</v>
+      </c>
+      <c r="B48" s="52">
+        <v>15.029478458049885</v>
+      </c>
+      <c r="C48" s="9">
+        <v>40.816326530612244</v>
+      </c>
+      <c r="D48" s="20">
+        <v>1</v>
+      </c>
+      <c r="E48" s="9">
+        <f t="shared" ref="E48:E50" si="8">B48*D48</f>
+        <v>15.029478458049885</v>
+      </c>
+      <c r="F48">
+        <v>428</v>
+      </c>
+      <c r="G48">
+        <v>270</v>
+      </c>
+      <c r="H48" s="9">
+        <f t="shared" ref="H48:H50" si="9">I48*60*C48/$B$44</f>
+        <v>9.1883696279300668</v>
+      </c>
+      <c r="I48" s="9">
+        <f>2*F48/G48</f>
+        <v>3.1703703703703705</v>
+      </c>
+      <c r="J48" s="9">
+        <f t="shared" ref="J48:J50" si="10">3.4+0.64*I48</f>
+        <v>5.4290370370370375</v>
+      </c>
+      <c r="K48" s="9">
+        <f t="shared" ref="K48:K50" si="11">$B$40*D48*$B$39*I48*C48*60/$B$3</f>
+        <v>183.76739255860136</v>
+      </c>
+      <c r="L48" s="9">
+        <f t="shared" ref="L48:L50" si="12">60*(24/$B$40 - 3.36*(F48/G48) - 5.9)</f>
+        <v>46.426666666666634</v>
+      </c>
+      <c r="M48" s="9">
+        <f t="shared" ref="M48:M50" si="13">H48/L48*60</f>
+        <v>11.874687916624161</v>
+      </c>
+    </row>
+    <row r="49" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>49</v>
+      </c>
+      <c r="B49" s="52">
+        <v>6.7437641723356005</v>
+      </c>
+      <c r="C49" s="9">
+        <v>95.238095238095241</v>
+      </c>
+      <c r="D49" s="20">
+        <v>20</v>
+      </c>
+      <c r="E49" s="9">
+        <f t="shared" si="8"/>
+        <v>134.87528344671202</v>
+      </c>
+      <c r="F49">
+        <v>300</v>
+      </c>
+      <c r="G49">
+        <v>550</v>
+      </c>
+      <c r="H49" s="9">
+        <f t="shared" si="9"/>
+        <v>7.3772381464689163</v>
+      </c>
+      <c r="I49" s="9">
+        <f>2*F49/G49</f>
+        <v>1.0909090909090908</v>
+      </c>
+      <c r="J49" s="9">
+        <f t="shared" si="10"/>
+        <v>4.0981818181818177</v>
+      </c>
+      <c r="K49" s="9">
+        <f t="shared" si="11"/>
+        <v>2950.8952585875659</v>
+      </c>
+      <c r="L49" s="9">
+        <f t="shared" si="12"/>
+        <v>256.03636363636366</v>
+      </c>
+      <c r="M49" s="9">
+        <f t="shared" si="13"/>
+        <v>1.7287946231605895</v>
+      </c>
+    </row>
+    <row r="50" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
+        <v>50</v>
+      </c>
+      <c r="B50" s="52">
+        <v>8.0535147392290245</v>
+      </c>
+      <c r="C50" s="9">
+        <v>8.2993197278911559</v>
+      </c>
+      <c r="D50" s="20">
+        <v>1</v>
+      </c>
+      <c r="E50" s="9">
+        <f t="shared" si="8"/>
+        <v>8.0535147392290245</v>
+      </c>
+      <c r="F50">
+        <v>200</v>
+      </c>
+      <c r="G50">
+        <v>120</v>
+      </c>
+      <c r="H50" s="9">
+        <f t="shared" si="9"/>
+        <v>1.9643360302700961</v>
+      </c>
+      <c r="I50" s="9">
+        <f>2*F50/G50</f>
+        <v>3.3333333333333335</v>
+      </c>
+      <c r="J50" s="9">
+        <f t="shared" si="10"/>
+        <v>5.5333333333333332</v>
+      </c>
+      <c r="K50" s="9">
+        <f t="shared" si="11"/>
+        <v>39.286720605401932</v>
+      </c>
+      <c r="L50" s="9">
+        <f t="shared" si="12"/>
+        <v>30</v>
+      </c>
+      <c r="M50" s="9">
+        <f t="shared" si="13"/>
+        <v>3.9286720605401917</v>
+      </c>
+    </row>
+    <row r="52" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B52" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C52" s="54">
+        <f>SUM(E47:E50)</f>
+        <v>171.25532879818596</v>
+      </c>
+      <c r="D52" t="s">
+        <v>10</v>
+      </c>
+      <c r="J52" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="K52" s="54">
+        <f>SUM(K47:K50)</f>
+        <v>3514.7137104227627</v>
+      </c>
+      <c r="L52" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="53" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="J53" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="K53" s="43">
+        <f>MAX(M47:M50)</f>
+        <v>11.874687916624161</v>
+      </c>
+      <c r="L53" s="2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="54" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B54" t="s">
+        <v>7</v>
+      </c>
+      <c r="C54" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="55" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A55" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B55" s="44">
+        <v>50</v>
+      </c>
+      <c r="C55" s="44">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="58" spans="1:14" ht="8.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A58" s="15"/>
+      <c r="B58" s="15"/>
+      <c r="C58" s="15"/>
+      <c r="D58" s="15"/>
+      <c r="E58" s="15"/>
+      <c r="F58" s="15"/>
+      <c r="G58" s="15"/>
+      <c r="H58" s="15"/>
+      <c r="I58" s="15"/>
+      <c r="J58" s="15"/>
+      <c r="K58" s="15"/>
+      <c r="L58" s="15"/>
+      <c r="M58" s="15"/>
+      <c r="N58" s="15"/>
+    </row>
+    <row r="59" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A59" t="s">
+        <v>123</v>
+      </c>
+      <c r="B59" t="s">
+        <v>129</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B16" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>